<commit_message>
Fix Kind dropdown for illumina and MGI.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_MGI_v5_3_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_MGI_v5_3_0.xlsx
@@ -11412,12 +11412,12 @@
       <formula1>Index!$L$2:$L$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E100" type="list">
-      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(INDEX(Index!$F$2:$F$4, MATCH(C7, Index!$E$2:$E$4, 0), 1), " ", "_"), "-", "_"))</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K100" type="list">
+      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(INDEX(Index!$J$2:$J$4, MATCH(C7, Index!$E$2:$E$4, 0), 1), " ", "_"), "-", "_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K7:K100" type="list">
-      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(INDEX(Index!$J$2:$J$4, MATCH(C7, Index!$E$2:$E$4, 0), 1), " ", "_"), "-", "_"))</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E7:E100" type="list">
+      <formula1>INDIRECT(SUBSTITUTE(SUBSTITUTE(INDEX(Index!$F$2:$F$4, MATCH(D7, Index!$E$2:$E$4, 0), 1), " ", "_"), "-", "_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>